<commit_message>
got excel a going
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519"/>
@@ -15,9 +15,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>I am title</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Case Number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Document Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>First Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Middle Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Last Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Suffix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Company Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Address 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Address 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>City</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>State</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zip</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -30,10 +78,6 @@
   </si>
   <si>
     <t>test4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pkp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -377,7 +421,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,28 +434,56 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2"/>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
@@ -422,8 +494,11 @@
       <c r="H3"/>
       <c r="I3"/>
       <c r="J3"/>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
@@ -434,8 +509,11 @@
       <c r="H4"/>
       <c r="I4"/>
       <c r="J4"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
@@ -446,8 +524,11 @@
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
@@ -458,8 +539,11 @@
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -470,8 +554,11 @@
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -482,8 +569,11 @@
       <c r="H8"/>
       <c r="I8"/>
       <c r="J8"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
@@ -494,8 +584,11 @@
       <c r="H9"/>
       <c r="I9"/>
       <c r="J9"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -506,8 +599,11 @@
       <c r="H10"/>
       <c r="I10"/>
       <c r="J10"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -518,8 +614,11 @@
       <c r="H11"/>
       <c r="I11"/>
       <c r="J11"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -530,6 +629,9 @@
       <c r="H12"/>
       <c r="I12"/>
       <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
got the first version working
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -7,7 +7,12 @@
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Consent Agreement" sheetId="1" r:id="rId1"/>
+    <sheet name="Final Notice Prior" sheetId="2" r:id="rId2"/>
+    <sheet name="UCVN" sheetId="3" r:id="rId3"/>
+    <sheet name="Enforcement Letter" sheetId="4" r:id="rId4"/>
+    <sheet name="Court" sheetId="5" r:id="rId5"/>
+    <sheet name="Enforcement Notice" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519"/>
@@ -15,33 +20,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Case Number</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Document Type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>First Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Middle Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Last Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Suffix</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Title</t>
+    <t>Owners Name(s)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -49,11 +34,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Address 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Address 2</t>
+    <t>Property Address 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Property Address 2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -69,15 +54,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>test2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test4</t>
+    <t>Mailing Address 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mailing Address 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEUNARINE DWARIKA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>   </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2431 N 61 AVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HOLLYWOOD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HABITAT FOR HUMANITY OF &amp; GREATER MIAMI INC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3800 NW 22 AVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIAMI</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -453,185 +466,417 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2"/>
+      <c r="A2" t="s">
+        <v>-1</v>
+      </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="J2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>-1</v>
+      </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
+      <c r="A3" t="s">
+        <v>-1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>-1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>-1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>-1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" t="s">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:13">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8"/>
-      <c r="M8"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-      <c r="M9"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
-      <c r="M11"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>-1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
got file naming correct
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -7,7 +7,9 @@
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
-    <sheet name="ENFORCEMENT LETTER" sheetId="1" r:id="rId1"/>
+    <sheet name="COURT" sheetId="1" r:id="rId1"/>
+    <sheet name="CONSENT AGREEMENT" sheetId="2" r:id="rId2"/>
+    <sheet name="ENFORCEMENT LETTER" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519"/>
@@ -15,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="261">
   <si>
     <t>Case Number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,6 +59,274 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>89-073</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GELIO HERNANDEZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HERNANDEZ GELIO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>   </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12401 W OKEECHOBEE RD #86</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hialeah</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>06-056</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEUNARINE DWARIKA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEACSU, MIHAI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2431 N 61 AVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HOLLYWOOD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TREE-07881</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REFERENCE ONLY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SUNCREST TOWNHOUSE CONDOMINIUM ASSOCIATION</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TREE-08216</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FESTER L LITTLE JR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FESTER LITTLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2441 NW 170 ST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miami Gardens</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>33056-4531</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2441  NW 170 ST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIAMI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TREE-08226</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JEFFREY OLIVER DAVIS JTRS &amp; JONATHAN DALE ANDERSON JTRS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JEFFREY DAVIS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>27278 SW 143 AVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unincorporated County</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>33032-8863</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HOMESTEAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16-106</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ANA ZOILA HERNANDEZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12025 NW 162 ST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>33018-0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>700 SW 31 AVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WWC-00001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CITY OF MIAMI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KEYSTONE TRAILER PARK </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6301 NE 2 AVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miami</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>33138-6016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>444 SW 2 AVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TREE-7723</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KENDALL LAKES  AUTOMOTIVE LLC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KENDALL LAKES AUTOMITIVE LLC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13355 SW 137 AVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>33186-5315</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16600 NW 57 AVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIAMI LAKES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLI-2017-0003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VICKI MILLER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MILLER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1444 W 28 ST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miami Beach</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>33140-4218</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIAMI BCH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DWO-00101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CITY OF HIALEAH GARDENS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CITY OF HIALEAH GARDENS (U5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10001 NW 87 AVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hialeah Gardens</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HIALEAH GARDENS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COM-72985</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WYNKEN-BLYNKEN &amp; NOD INC &amp; % SBL REALTY CO INC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRAILER PARK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12401 W OKEECHOBEE RD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>501 BRICKELL KEY DR #103</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>PSO-00413</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -73,22 +343,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Unincorporated County</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>777 BRICKELL AVE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MIAMI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>IW5-01764</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -181,26 +439,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>HOMESTEAD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>IW5-13201</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>REFERENCE ONLY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>NATIONAL LIFT TRUCK SERVICE INC.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>   </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>IW5-15756</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -321,10 +567,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Miami</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>33142-7114</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -581,10 +823,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Miami Gardens</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>33054-2466</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -609,10 +847,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Hialeah</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>33013-3524</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -746,10 +980,6 @@
   </si>
   <si>
     <t>17801 NW 137 AVE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HIALEAH GARDENS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1231,25 +1461,25 @@
         <v>-1</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>-1</v>
       </c>
       <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
-        <v>-1</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
-        <v>-1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
-      </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M2" t="s">
         <v>-1</v>
@@ -1257,40 +1487,40 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>-1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>-1</v>
+      </c>
+      <c r="I3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="J3" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
-        <v>-1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>-1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
-      </c>
       <c r="L3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M3" t="s">
         <v>-1</v>
@@ -1298,40 +1528,219 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>-1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>-1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" t="s">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
         <v>24</v>
       </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" t="s">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
         <v>-1</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
         <v>-1</v>
       </c>
       <c r="K4" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="L4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M4" t="s">
         <v>-1</v>
@@ -1339,40 +1748,40 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K5" t="s">
         <v>32</v>
       </c>
-      <c r="E5" t="s">
-        <v>-1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" t="s">
-        <v>-1</v>
-      </c>
-      <c r="K5" t="s">
-        <v>17</v>
-      </c>
       <c r="L5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M5" t="s">
         <v>-1</v>
@@ -1380,40 +1789,40 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
         <v>-1</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J6" t="s">
         <v>-1</v>
       </c>
       <c r="K6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="L6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M6" t="s">
         <v>-1</v>
@@ -1421,40 +1830,40 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
         <v>-1</v>
       </c>
       <c r="F7" t="s">
-        <v>-1</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>-1</v>
+        <v>56</v>
       </c>
       <c r="I7" t="s">
-        <v>-1</v>
+        <v>57</v>
       </c>
       <c r="J7" t="s">
         <v>-1</v>
       </c>
       <c r="K7" t="s">
-        <v>-1</v>
+        <v>58</v>
       </c>
       <c r="L7" t="s">
-        <v>-1</v>
+        <v>14</v>
       </c>
       <c r="M7" t="s">
         <v>-1</v>
@@ -1462,40 +1871,40 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
         <v>-1</v>
       </c>
       <c r="F8" t="s">
-        <v>-1</v>
+        <v>63</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>-1</v>
+        <v>64</v>
       </c>
       <c r="I8" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="J8" t="s">
         <v>-1</v>
       </c>
       <c r="K8" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="L8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M8" t="s">
         <v>-1</v>
@@ -1503,40 +1912,40 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
         <v>-1</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
+        <v>-1</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="J9" t="s">
         <v>-1</v>
       </c>
       <c r="K9" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="L9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M9" t="s">
         <v>-1</v>
@@ -1544,40 +1953,465 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="E10" t="s">
         <v>-1</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="I10" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="J10" t="s">
         <v>-1</v>
       </c>
       <c r="K10" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="L10" t="s">
-        <v>63</v>
+        <v>14</v>
+      </c>
+      <c r="M10" t="s">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" t="s">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" t="s">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J5" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" t="s">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" t="s">
+        <v>104</v>
+      </c>
+      <c r="J6" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" t="s">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>-1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>-1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>-1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>-1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>-1</v>
+      </c>
+      <c r="M7" t="s">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>-1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>-1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>110</v>
+      </c>
+      <c r="J8" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" t="s">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>115</v>
+      </c>
+      <c r="I9" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" t="s">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" t="s">
+        <v>-1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>121</v>
+      </c>
+      <c r="I10" t="s">
+        <v>122</v>
+      </c>
+      <c r="J10" t="s">
+        <v>-1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>123</v>
+      </c>
+      <c r="L10" t="s">
+        <v>124</v>
       </c>
       <c r="M10" t="s">
         <v>-1</v>
@@ -1585,40 +2419,40 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>127</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>128</v>
       </c>
       <c r="E11" t="s">
         <v>-1</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" t="s">
-        <v>68</v>
+        <v>129</v>
       </c>
       <c r="I11" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="J11" t="s">
         <v>-1</v>
       </c>
       <c r="K11" t="s">
-        <v>70</v>
+        <v>131</v>
       </c>
       <c r="L11" t="s">
-        <v>71</v>
+        <v>132</v>
       </c>
       <c r="M11" t="s">
         <v>-1</v>
@@ -1626,40 +2460,40 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>134</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>135</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="E12" t="s">
         <v>-1</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" t="s">
-        <v>77</v>
+        <v>137</v>
       </c>
       <c r="I12" t="s">
-        <v>78</v>
+        <v>138</v>
       </c>
       <c r="J12" t="s">
         <v>-1</v>
       </c>
       <c r="K12" t="s">
-        <v>79</v>
+        <v>139</v>
       </c>
       <c r="L12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M12" t="s">
         <v>-1</v>
@@ -1667,40 +2501,40 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>142</v>
       </c>
       <c r="D13" t="s">
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="E13" t="s">
         <v>-1</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" t="s">
-        <v>84</v>
+        <v>144</v>
       </c>
       <c r="I13" t="s">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="J13" t="s">
         <v>-1</v>
       </c>
       <c r="K13" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="L13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M13" t="s">
         <v>-1</v>
@@ -1708,40 +2542,40 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>146</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>148</v>
       </c>
       <c r="D14" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="E14" t="s">
         <v>-1</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14" t="s">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="I14" t="s">
-        <v>91</v>
+        <v>151</v>
       </c>
       <c r="J14" t="s">
         <v>-1</v>
       </c>
       <c r="K14" t="s">
-        <v>92</v>
+        <v>152</v>
       </c>
       <c r="L14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M14" t="s">
         <v>-1</v>
@@ -1749,40 +2583,40 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>153</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>154</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
+        <v>155</v>
       </c>
       <c r="D15" t="s">
-        <v>96</v>
+        <v>156</v>
       </c>
       <c r="E15" t="s">
         <v>-1</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15" t="s">
-        <v>97</v>
+        <v>157</v>
       </c>
       <c r="I15" t="s">
-        <v>98</v>
+        <v>158</v>
       </c>
       <c r="J15" t="s">
         <v>-1</v>
       </c>
       <c r="K15" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="L15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M15" t="s">
         <v>-1</v>
@@ -1790,40 +2624,40 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>159</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>161</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>162</v>
       </c>
       <c r="E16" t="s">
         <v>-1</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="G16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>103</v>
+        <v>163</v>
       </c>
       <c r="I16" t="s">
-        <v>102</v>
+        <v>162</v>
       </c>
       <c r="J16" t="s">
         <v>-1</v>
       </c>
       <c r="K16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M16" t="s">
         <v>-1</v>
@@ -1831,40 +2665,40 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>164</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>165</v>
       </c>
       <c r="C17" t="s">
-        <v>106</v>
+        <v>166</v>
       </c>
       <c r="D17" t="s">
-        <v>107</v>
+        <v>167</v>
       </c>
       <c r="E17" t="s">
         <v>-1</v>
       </c>
       <c r="F17" t="s">
-        <v>108</v>
+        <v>168</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17" t="s">
-        <v>109</v>
+        <v>169</v>
       </c>
       <c r="I17" t="s">
-        <v>110</v>
+        <v>170</v>
       </c>
       <c r="J17" t="s">
         <v>-1</v>
       </c>
       <c r="K17" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="L17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M17" t="s">
         <v>-1</v>
@@ -1872,16 +2706,16 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>172</v>
       </c>
       <c r="C18" t="s">
-        <v>112</v>
+        <v>172</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
         <v>-1</v>
@@ -1890,22 +2724,22 @@
         <v>-1</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H18" t="s">
         <v>-1</v>
       </c>
       <c r="I18" t="s">
-        <v>113</v>
+        <v>173</v>
       </c>
       <c r="J18" t="s">
         <v>-1</v>
       </c>
       <c r="K18" t="s">
-        <v>114</v>
+        <v>174</v>
       </c>
       <c r="L18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M18" t="s">
         <v>-1</v>
@@ -1913,40 +2747,40 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>115</v>
+        <v>175</v>
       </c>
       <c r="B19" t="s">
-        <v>116</v>
+        <v>176</v>
       </c>
       <c r="C19" t="s">
-        <v>117</v>
+        <v>177</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>178</v>
       </c>
       <c r="E19" t="s">
         <v>-1</v>
       </c>
       <c r="F19" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s">
-        <v>119</v>
+        <v>179</v>
       </c>
       <c r="I19" t="s">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="J19" t="s">
         <v>-1</v>
       </c>
       <c r="K19" t="s">
-        <v>121</v>
+        <v>181</v>
       </c>
       <c r="L19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M19" t="s">
         <v>-1</v>
@@ -1954,40 +2788,40 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>182</v>
       </c>
       <c r="B20" t="s">
-        <v>123</v>
+        <v>183</v>
       </c>
       <c r="C20" t="s">
-        <v>124</v>
+        <v>184</v>
       </c>
       <c r="D20" t="s">
-        <v>125</v>
+        <v>185</v>
       </c>
       <c r="E20" t="s">
         <v>-1</v>
       </c>
       <c r="F20" t="s">
-        <v>126</v>
+        <v>186</v>
       </c>
       <c r="G20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H20" t="s">
-        <v>127</v>
+        <v>187</v>
       </c>
       <c r="I20" t="s">
-        <v>128</v>
+        <v>188</v>
       </c>
       <c r="J20" t="s">
         <v>-1</v>
       </c>
       <c r="K20" t="s">
-        <v>129</v>
+        <v>189</v>
       </c>
       <c r="L20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M20" t="s">
         <v>-1</v>
@@ -1995,40 +2829,40 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>130</v>
+        <v>190</v>
       </c>
       <c r="B21" t="s">
-        <v>131</v>
+        <v>191</v>
       </c>
       <c r="C21" t="s">
-        <v>132</v>
+        <v>192</v>
       </c>
       <c r="D21" t="s">
-        <v>133</v>
+        <v>193</v>
       </c>
       <c r="E21" t="s">
         <v>-1</v>
       </c>
       <c r="F21" t="s">
-        <v>108</v>
+        <v>168</v>
       </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" t="s">
-        <v>134</v>
+        <v>194</v>
       </c>
       <c r="I21" t="s">
-        <v>135</v>
+        <v>195</v>
       </c>
       <c r="J21" t="s">
         <v>-1</v>
       </c>
       <c r="K21" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="L21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M21" t="s">
         <v>-1</v>
@@ -2036,40 +2870,40 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>197</v>
       </c>
       <c r="B22" t="s">
-        <v>138</v>
+        <v>198</v>
       </c>
       <c r="C22" t="s">
-        <v>139</v>
+        <v>199</v>
       </c>
       <c r="D22" t="s">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="E22" t="s">
         <v>-1</v>
       </c>
       <c r="F22" t="s">
-        <v>141</v>
+        <v>29</v>
       </c>
       <c r="G22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H22" t="s">
-        <v>142</v>
+        <v>201</v>
       </c>
       <c r="I22" t="s">
-        <v>143</v>
+        <v>202</v>
       </c>
       <c r="J22" t="s">
         <v>-1</v>
       </c>
       <c r="K22" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="L22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M22" t="s">
         <v>-1</v>
@@ -2077,40 +2911,40 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>144</v>
+        <v>203</v>
       </c>
       <c r="B23" t="s">
-        <v>145</v>
+        <v>204</v>
       </c>
       <c r="C23" t="s">
-        <v>146</v>
+        <v>205</v>
       </c>
       <c r="D23" t="s">
-        <v>147</v>
+        <v>206</v>
       </c>
       <c r="E23" t="s">
         <v>-1</v>
       </c>
       <c r="F23" t="s">
-        <v>148</v>
+        <v>16</v>
       </c>
       <c r="G23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H23" t="s">
-        <v>149</v>
+        <v>207</v>
       </c>
       <c r="I23" t="s">
-        <v>150</v>
+        <v>208</v>
       </c>
       <c r="J23" t="s">
         <v>-1</v>
       </c>
       <c r="K23" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="L23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M23" t="s">
         <v>-1</v>
@@ -2118,40 +2952,40 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>151</v>
+        <v>209</v>
       </c>
       <c r="B24" t="s">
-        <v>152</v>
+        <v>210</v>
       </c>
       <c r="C24" t="s">
-        <v>153</v>
+        <v>211</v>
       </c>
       <c r="D24" t="s">
-        <v>154</v>
+        <v>212</v>
       </c>
       <c r="E24" t="s">
         <v>-1</v>
       </c>
       <c r="F24" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="G24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H24" t="s">
         <v>-1</v>
       </c>
       <c r="I24" t="s">
-        <v>155</v>
+        <v>213</v>
       </c>
       <c r="J24" t="s">
         <v>-1</v>
       </c>
       <c r="K24" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="L24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M24" t="s">
         <v>-1</v>
@@ -2159,40 +2993,40 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" t="s">
-        <v>156</v>
+        <v>214</v>
       </c>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>215</v>
       </c>
       <c r="C25" t="s">
-        <v>158</v>
+        <v>216</v>
       </c>
       <c r="D25" t="s">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="E25" t="s">
         <v>-1</v>
       </c>
       <c r="F25" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="G25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H25" t="s">
-        <v>160</v>
+        <v>218</v>
       </c>
       <c r="I25" t="s">
-        <v>161</v>
+        <v>219</v>
       </c>
       <c r="J25" t="s">
         <v>-1</v>
       </c>
       <c r="K25" t="s">
-        <v>162</v>
+        <v>220</v>
       </c>
       <c r="L25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M25" t="s">
         <v>-1</v>
@@ -2200,40 +3034,40 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
-        <v>163</v>
+        <v>221</v>
       </c>
       <c r="B26" t="s">
-        <v>164</v>
+        <v>222</v>
       </c>
       <c r="C26" t="s">
-        <v>165</v>
+        <v>223</v>
       </c>
       <c r="D26" t="s">
-        <v>166</v>
+        <v>224</v>
       </c>
       <c r="E26" t="s">
         <v>-1</v>
       </c>
       <c r="F26" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="G26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H26" t="s">
-        <v>167</v>
+        <v>225</v>
       </c>
       <c r="I26" t="s">
-        <v>168</v>
+        <v>226</v>
       </c>
       <c r="J26" t="s">
         <v>-1</v>
       </c>
       <c r="K26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M26" t="s">
         <v>-1</v>
@@ -2241,40 +3075,40 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>227</v>
       </c>
       <c r="B27" t="s">
-        <v>170</v>
+        <v>228</v>
       </c>
       <c r="C27" t="s">
-        <v>171</v>
+        <v>229</v>
       </c>
       <c r="D27" t="s">
-        <v>172</v>
+        <v>230</v>
       </c>
       <c r="E27" t="s">
         <v>-1</v>
       </c>
       <c r="F27" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="G27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H27" t="s">
-        <v>173</v>
+        <v>231</v>
       </c>
       <c r="I27" t="s">
-        <v>174</v>
+        <v>232</v>
       </c>
       <c r="J27" t="s">
         <v>-1</v>
       </c>
       <c r="K27" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="L27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M27" t="s">
         <v>-1</v>
@@ -2282,16 +3116,16 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" t="s">
-        <v>175</v>
+        <v>233</v>
       </c>
       <c r="B28" t="s">
-        <v>176</v>
+        <v>234</v>
       </c>
       <c r="C28" t="s">
-        <v>176</v>
+        <v>234</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="E28" t="s">
         <v>-1</v>
@@ -2300,22 +3134,22 @@
         <v>-1</v>
       </c>
       <c r="G28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H28" t="s">
         <v>-1</v>
       </c>
       <c r="I28" t="s">
-        <v>177</v>
+        <v>235</v>
       </c>
       <c r="J28" t="s">
         <v>-1</v>
       </c>
       <c r="K28" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="L28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M28" t="s">
         <v>-1</v>
@@ -2323,40 +3157,40 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" t="s">
-        <v>178</v>
+        <v>236</v>
       </c>
       <c r="B29" t="s">
-        <v>179</v>
+        <v>237</v>
       </c>
       <c r="C29" t="s">
-        <v>179</v>
+        <v>237</v>
       </c>
       <c r="D29" t="s">
-        <v>180</v>
+        <v>238</v>
       </c>
       <c r="E29" t="s">
         <v>-1</v>
       </c>
       <c r="F29" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H29" t="s">
-        <v>181</v>
+        <v>239</v>
       </c>
       <c r="I29" t="s">
-        <v>182</v>
+        <v>240</v>
       </c>
       <c r="J29" t="s">
         <v>-1</v>
       </c>
       <c r="K29" t="s">
-        <v>183</v>
+        <v>71</v>
       </c>
       <c r="L29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M29" t="s">
         <v>-1</v>
@@ -2364,40 +3198,40 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" t="s">
-        <v>184</v>
+        <v>241</v>
       </c>
       <c r="B30" t="s">
-        <v>185</v>
+        <v>242</v>
       </c>
       <c r="C30" t="s">
-        <v>186</v>
+        <v>243</v>
       </c>
       <c r="D30" t="s">
-        <v>187</v>
+        <v>244</v>
       </c>
       <c r="E30" t="s">
         <v>-1</v>
       </c>
       <c r="F30" t="s">
-        <v>148</v>
+        <v>16</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H30" t="s">
-        <v>188</v>
+        <v>245</v>
       </c>
       <c r="I30" t="s">
-        <v>189</v>
+        <v>246</v>
       </c>
       <c r="J30" t="s">
         <v>-1</v>
       </c>
       <c r="K30" t="s">
-        <v>121</v>
+        <v>181</v>
       </c>
       <c r="L30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M30" t="s">
         <v>-1</v>
@@ -2405,40 +3239,40 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>190</v>
+        <v>247</v>
       </c>
       <c r="B31" t="s">
-        <v>191</v>
+        <v>248</v>
       </c>
       <c r="C31" t="s">
-        <v>192</v>
+        <v>249</v>
       </c>
       <c r="D31" t="s">
-        <v>193</v>
+        <v>250</v>
       </c>
       <c r="E31" t="s">
         <v>-1</v>
       </c>
       <c r="F31" t="s">
-        <v>194</v>
+        <v>251</v>
       </c>
       <c r="G31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H31" t="s">
-        <v>195</v>
+        <v>252</v>
       </c>
       <c r="I31" t="s">
-        <v>196</v>
+        <v>253</v>
       </c>
       <c r="J31" t="s">
         <v>-1</v>
       </c>
       <c r="K31" t="s">
-        <v>197</v>
+        <v>254</v>
       </c>
       <c r="L31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M31" t="s">
         <v>-1</v>
@@ -2446,40 +3280,40 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>198</v>
+        <v>255</v>
       </c>
       <c r="B32" t="s">
-        <v>199</v>
+        <v>256</v>
       </c>
       <c r="C32" t="s">
-        <v>200</v>
+        <v>257</v>
       </c>
       <c r="D32" t="s">
-        <v>201</v>
+        <v>258</v>
       </c>
       <c r="E32" t="s">
         <v>-1</v>
       </c>
       <c r="F32" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="G32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H32" t="s">
-        <v>202</v>
+        <v>259</v>
       </c>
       <c r="I32" t="s">
-        <v>203</v>
+        <v>260</v>
       </c>
       <c r="J32" t="s">
         <v>-1</v>
       </c>
       <c r="K32" t="s">
-        <v>92</v>
+        <v>152</v>
       </c>
       <c r="L32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M32" t="s">
         <v>-1</v>

</xml_diff>